<commit_message>
Mudança no background da aplicação
</commit_message>
<xml_diff>
--- a/_dados/Teste Clientes.xlsx
+++ b/_dados/Teste Clientes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ti04\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sorteio-pague-pouco\_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FAF085-841F-457D-B3E4-F655E26305CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A39C9A-F7E4-46BA-AD95-4E0144A592EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1123,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>